<commit_message>
xg boost predictions addded and other minor changes
</commit_message>
<xml_diff>
--- a/models-accuracy.xlsx
+++ b/models-accuracy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kusha\Desktop\Flipkart-Category-Prediction-NLP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{579BCCA5-89A7-465F-B696-94C85A918175}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904EB887-E129-41E7-9462-679AACD85612}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{56A13173-9D1B-481D-8F8D-4E180F63070C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Multinomial Naive Bayes (Count Vectorizer)</t>
   </si>
@@ -45,12 +45,6 @@
     <t>Random Forest Classifier (TF-IDF Vectorizer)</t>
   </si>
   <si>
-    <t>Gradient Boosting Classifier (Count Vectorizer + TfidfVectorizer)</t>
-  </si>
-  <si>
-    <t>KNeighbours Classifier (Count Vectorizer + TfidfVectorizer)</t>
-  </si>
-  <si>
     <t>Model Name</t>
   </si>
   <si>
@@ -60,7 +54,25 @@
     <t>Training Accuracy</t>
   </si>
   <si>
-    <t>Cross Validation Accuracy</t>
+    <t>Cross Validation Mean Accuracy</t>
+  </si>
+  <si>
+    <t>Gradient Boosting Classifier (Count Vectorizer + TfidfTransformer)</t>
+  </si>
+  <si>
+    <t>KNeighbours Classifier (Count Vectorizer + TfidfTransformer)</t>
+  </si>
+  <si>
+    <t>Gradient Boosting Classifier (Count Vectorizer)</t>
+  </si>
+  <si>
+    <t>KNeighbours Classifier (Count Vectorizer)</t>
+  </si>
+  <si>
+    <t>Xgboost Classifier (Count Vectorizer)</t>
+  </si>
+  <si>
+    <t>Xgboost Classifier (Count Vectorizer + TfidfTransformer)</t>
   </si>
 </sst>
 </file>
@@ -421,15 +433,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEEE7161-8079-4663-A31F-DDAB933D0DD2}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="53.33203125" customWidth="1"/>
+    <col min="1" max="1" width="55.5546875" customWidth="1"/>
     <col min="2" max="2" width="19.109375" customWidth="1"/>
     <col min="3" max="3" width="16.5546875" customWidth="1"/>
     <col min="4" max="4" width="28.109375" customWidth="1"/>
@@ -437,16 +449,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -535,30 +547,69 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>0.75343162175902301</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0.78241800152555296</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0.58827413057890998</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B9" s="1">
+        <v>0.75343162175902301</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.78241800152555296</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.58827413057890998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.95907473309608504</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.99885583524027399</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
         <v>0.95729537366548001</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C11" s="1">
         <v>0.99872870582252704</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D11" s="1">
         <v>0.90801427210297103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.97458057956278599</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.99771167048054898</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.97127605490594804</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.99879227053140096</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
report added and other minor changes
</commit_message>
<xml_diff>
--- a/models-accuracy.xlsx
+++ b/models-accuracy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kusha\Desktop\Flipkart-Category-Prediction-NLP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904EB887-E129-41E7-9462-679AACD85612}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9813F7-C9FB-493B-A012-4B2750F1A33E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{56A13173-9D1B-481D-8F8D-4E180F63070C}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>Training Accuracy</t>
   </si>
   <si>
-    <t>Cross Validation Mean Accuracy</t>
-  </si>
-  <si>
     <t>Gradient Boosting Classifier (Count Vectorizer + TfidfTransformer)</t>
   </si>
   <si>
@@ -73,6 +70,9 @@
   </si>
   <si>
     <t>Xgboost Classifier (Count Vectorizer + TfidfTransformer)</t>
+  </si>
+  <si>
+    <t>Mean Cross Validation Accuracy</t>
   </si>
 </sst>
 </file>
@@ -436,7 +436,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -458,7 +458,7 @@
         <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -547,12 +547,21 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.91916624300965899</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.94457157386219104</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.83082393952284905</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1">
         <v>0.75343162175902301</v>
@@ -566,7 +575,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1">
         <v>0.95907473309608504</v>
@@ -574,11 +583,13 @@
       <c r="C10" s="1">
         <v>0.99885583524027399</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="1">
+        <v>0.90318344471214596</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1">
         <v>0.95729537366548001</v>
@@ -592,7 +603,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1">
         <v>0.97458057956278599</v>
@@ -600,16 +611,22 @@
       <c r="C12" s="1">
         <v>0.99771167048054898</v>
       </c>
+      <c r="D12" s="1">
+        <v>0.93089596444564304</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="1">
         <v>0.97127605490594804</v>
       </c>
       <c r="C13" s="1">
         <v>0.99879227053140096</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.92825155622047995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>